<commit_message>
added new info to levine
</commit_message>
<xml_diff>
--- a/dna-methylation/routines/levine.xlsx
+++ b/dna-methylation/routines/levine.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Гаврилов Аркадий Сергеевич</t>
   </si>
@@ -151,6 +151,27 @@
   </si>
   <si>
     <t>F1L15</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>MQ1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>MQ2</t>
+  </si>
+  <si>
+    <t>SQ2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>MQ3</t>
   </si>
 </sst>
 </file>
@@ -160,7 +181,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd\.mm"/>
     <numFmt numFmtId="165" formatCode="d\.m"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -255,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -275,7 +296,7 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -310,6 +331,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,17 +618,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AH34"/>
+  <dimension ref="A1:AH41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="B35" sqref="B35:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" style="3"/>
-    <col min="2" max="2" width="24" style="11"/>
-    <col min="3" max="16384" width="24" style="3"/>
+    <col min="2" max="3" width="24" style="11"/>
+    <col min="4" max="16384" width="24" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -614,7 +638,7 @@
       <c r="B1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -656,7 +680,7 @@
       <c r="B2" s="10">
         <v>92</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="10">
         <v>44.4</v>
       </c>
       <c r="D2" s="7">
@@ -712,7 +736,7 @@
       <c r="B3" s="10">
         <v>90</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="10">
         <v>46.5</v>
       </c>
       <c r="D3" s="7">
@@ -769,7 +793,7 @@
       <c r="B4" s="10">
         <v>61</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="10">
         <v>40.799999999999997</v>
       </c>
       <c r="D4" s="7">
@@ -826,7 +850,7 @@
       <c r="B5" s="10">
         <v>28</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="10">
         <v>42.6</v>
       </c>
       <c r="D5" s="7">
@@ -883,7 +907,7 @@
       <c r="B6" s="10">
         <v>32</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="10">
         <v>46</v>
       </c>
       <c r="D6" s="7">
@@ -940,7 +964,7 @@
       <c r="B7" s="10">
         <v>68</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="10">
         <v>39.700000000000003</v>
       </c>
       <c r="D7" s="7">
@@ -997,7 +1021,7 @@
       <c r="B8" s="10">
         <v>37</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="10">
         <v>52.2</v>
       </c>
       <c r="D8" s="7">
@@ -1054,7 +1078,7 @@
       <c r="B9" s="10">
         <v>41</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="10">
         <v>58.5</v>
       </c>
       <c r="D9" s="7">
@@ -1111,7 +1135,7 @@
       <c r="B10" s="10">
         <v>15</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="10">
         <v>42.9</v>
       </c>
       <c r="D10" s="7">
@@ -1168,7 +1192,7 @@
       <c r="B11" s="10">
         <v>91</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="10">
         <v>40.9</v>
       </c>
       <c r="D11" s="7">
@@ -1224,7 +1248,7 @@
       <c r="B12" s="10">
         <v>65</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="10">
         <v>38.9</v>
       </c>
       <c r="D12" s="7">
@@ -1280,7 +1304,7 @@
       <c r="B13" s="10">
         <v>43</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="10">
         <v>24.8</v>
       </c>
       <c r="D13" s="7">
@@ -1336,7 +1360,7 @@
       <c r="B14" s="10">
         <v>88</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="10">
         <v>48.1</v>
       </c>
       <c r="D14" s="7">
@@ -1393,7 +1417,7 @@
       <c r="B15" s="10">
         <v>57</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="10">
         <v>56.7</v>
       </c>
       <c r="D15" s="7">
@@ -1450,7 +1474,7 @@
       <c r="B16" s="10">
         <v>87</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="10">
         <v>42.1</v>
       </c>
       <c r="D16" s="7">
@@ -1507,7 +1531,7 @@
       <c r="B17" s="10">
         <v>63</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="10">
         <v>57.9</v>
       </c>
       <c r="D17" s="7">
@@ -1564,7 +1588,7 @@
       <c r="B18" s="10">
         <v>39</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="10">
         <v>53.9</v>
       </c>
       <c r="D18" s="7">
@@ -1621,7 +1645,7 @@
       <c r="B19" s="10">
         <v>96</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="10">
         <v>23.8</v>
       </c>
       <c r="D19" s="7">
@@ -1678,7 +1702,7 @@
       <c r="B20" s="10">
         <v>59</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="10">
         <v>46.8</v>
       </c>
       <c r="D20" s="7">
@@ -1735,7 +1759,7 @@
       <c r="B21" s="10">
         <v>36</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="10">
         <v>50</v>
       </c>
       <c r="D21" s="7">
@@ -1792,7 +1816,7 @@
       <c r="B22" s="10">
         <v>93</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="10">
         <v>41</v>
       </c>
       <c r="D22" s="1">
@@ -1848,7 +1872,7 @@
       <c r="B23" s="10">
         <v>64</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="10">
         <v>34.4</v>
       </c>
       <c r="D23" s="1">
@@ -1904,7 +1928,7 @@
       <c r="B24" s="10">
         <v>94</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="10">
         <v>36.5</v>
       </c>
       <c r="D24" s="1">
@@ -1960,7 +1984,7 @@
       <c r="B25" s="10">
         <v>66</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="10">
         <v>35.1</v>
       </c>
       <c r="D25" s="1">
@@ -2016,7 +2040,7 @@
       <c r="B26" s="10">
         <v>91</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="10">
         <v>27.8</v>
       </c>
       <c r="D26" s="1">
@@ -2073,7 +2097,7 @@
       <c r="B27" s="10">
         <v>69</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="10">
         <v>26</v>
       </c>
       <c r="D27" s="1">
@@ -2130,7 +2154,7 @@
       <c r="B28" s="11">
         <v>0</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="10">
         <v>69.099999999999994</v>
       </c>
       <c r="D28" s="1">
@@ -2186,7 +2210,7 @@
       <c r="B29" s="11">
         <v>86</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="11">
         <v>35.1</v>
       </c>
       <c r="D29" s="3">
@@ -2221,7 +2245,7 @@
       <c r="B30" s="11">
         <v>32</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="11">
         <v>61.3</v>
       </c>
       <c r="D30" s="3">
@@ -2256,7 +2280,7 @@
       <c r="B31" s="11">
         <v>94</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="11">
         <v>45.6</v>
       </c>
       <c r="D31" s="3">
@@ -2291,7 +2315,7 @@
       <c r="B32" s="11">
         <v>0</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="11">
         <v>48.1</v>
       </c>
       <c r="D32" s="3">
@@ -2326,7 +2350,7 @@
       <c r="B33" s="11">
         <v>91</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="11">
         <v>36.6</v>
       </c>
       <c r="D33" s="3">
@@ -2361,7 +2385,7 @@
       <c r="B34" s="11">
         <v>65</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="11">
         <v>18.7</v>
       </c>
       <c r="D34" s="3">
@@ -2387,6 +2411,251 @@
       </c>
       <c r="K34" s="3">
         <v>11.49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="11">
+        <v>4</v>
+      </c>
+      <c r="C35" s="11">
+        <v>60.4</v>
+      </c>
+      <c r="D35" s="3">
+        <v>50.6</v>
+      </c>
+      <c r="E35" s="3">
+        <v>7.93</v>
+      </c>
+      <c r="F35" s="3">
+        <v>82</v>
+      </c>
+      <c r="G35" s="3">
+        <v>53.3</v>
+      </c>
+      <c r="H35" s="3">
+        <v>102</v>
+      </c>
+      <c r="I35" s="3">
+        <v>14.8</v>
+      </c>
+      <c r="J35" s="3">
+        <v>445</v>
+      </c>
+      <c r="K35" s="3">
+        <v>6.02</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="11">
+        <v>46</v>
+      </c>
+      <c r="C36" s="11">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="D36" s="3">
+        <v>60.2</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1.95</v>
+      </c>
+      <c r="F36" s="3">
+        <v>87.5</v>
+      </c>
+      <c r="G36" s="3">
+        <v>40</v>
+      </c>
+      <c r="H36" s="3">
+        <v>111</v>
+      </c>
+      <c r="I36" s="3">
+        <v>14.3</v>
+      </c>
+      <c r="J36" s="3">
+        <v>157</v>
+      </c>
+      <c r="K36" s="3">
+        <v>5.28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="11">
+        <v>8</v>
+      </c>
+      <c r="C37" s="11">
+        <v>57</v>
+      </c>
+      <c r="D37" s="3">
+        <v>28.4</v>
+      </c>
+      <c r="E37" s="3">
+        <v>5.64</v>
+      </c>
+      <c r="F37" s="3">
+        <v>89.5</v>
+      </c>
+      <c r="G37" s="3">
+        <v>15.3</v>
+      </c>
+      <c r="H37" s="3">
+        <v>95</v>
+      </c>
+      <c r="I37" s="3">
+        <v>13.3</v>
+      </c>
+      <c r="J37" s="3">
+        <v>501</v>
+      </c>
+      <c r="K37" s="3">
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="11">
+        <v>45</v>
+      </c>
+      <c r="C38" s="11">
+        <v>62.6</v>
+      </c>
+      <c r="D38" s="3">
+        <v>29.1</v>
+      </c>
+      <c r="E38" s="3">
+        <v>3.29</v>
+      </c>
+      <c r="F38" s="3">
+        <v>168.7</v>
+      </c>
+      <c r="G38" s="3">
+        <v>21.6</v>
+      </c>
+      <c r="H38" s="3">
+        <v>108</v>
+      </c>
+      <c r="I38" s="3">
+        <v>11.8</v>
+      </c>
+      <c r="J38" s="3">
+        <v>155</v>
+      </c>
+      <c r="K38" s="3">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="11">
+        <v>14</v>
+      </c>
+      <c r="C39" s="11">
+        <v>37</v>
+      </c>
+      <c r="D39" s="3">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="E39" s="3">
+        <v>4.37</v>
+      </c>
+      <c r="F39" s="3">
+        <v>103.1</v>
+      </c>
+      <c r="G39" s="3">
+        <v>27.3</v>
+      </c>
+      <c r="H39" s="3">
+        <v>99</v>
+      </c>
+      <c r="I39" s="3">
+        <v>12.9</v>
+      </c>
+      <c r="J39" s="3">
+        <v>397.9</v>
+      </c>
+      <c r="K39" s="3">
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="11">
+        <v>5</v>
+      </c>
+      <c r="C40" s="11">
+        <v>27.9</v>
+      </c>
+      <c r="D40" s="3">
+        <v>87.3</v>
+      </c>
+      <c r="E40" s="3">
+        <v>5.15</v>
+      </c>
+      <c r="F40" s="3">
+        <v>89</v>
+      </c>
+      <c r="G40" s="3">
+        <v>28.5</v>
+      </c>
+      <c r="H40" s="3">
+        <v>101</v>
+      </c>
+      <c r="I40" s="3">
+        <v>13</v>
+      </c>
+      <c r="J40" s="3">
+        <v>402.6</v>
+      </c>
+      <c r="K40" s="3">
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="11">
+        <v>43</v>
+      </c>
+      <c r="C41" s="11">
+        <v>27.3</v>
+      </c>
+      <c r="D41" s="3">
+        <v>88</v>
+      </c>
+      <c r="E41" s="3">
+        <v>4.57</v>
+      </c>
+      <c r="F41" s="3">
+        <v>61</v>
+      </c>
+      <c r="G41" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="H41" s="3">
+        <v>109</v>
+      </c>
+      <c r="I41" s="3">
+        <v>12.8</v>
+      </c>
+      <c r="J41" s="3">
+        <v>179.2</v>
+      </c>
+      <c r="K41" s="3">
+        <v>8.7100000000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>